<commit_message>
modified the links for PPTs
</commit_message>
<xml_diff>
--- a/Springer Nature/advanceml/PPTs.xlsx
+++ b/Springer Nature/advanceml/PPTs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Machine_Learning_Training\Springer Nature\advanceml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1831CDCB-9D45-4723-BBC4-2F6818FD68FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C29759-FFB4-4D92-BC22-EEBDADFF4FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="1620" windowWidth="19215" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>https://github.com/anshupandey/Computer-Vision/blob/master/Neural%20Networks%20and%20CNN/ANN%20Basics.pptx</t>
   </si>
@@ -43,16 +43,54 @@
   </si>
   <si>
     <t>https://github.com/anshupandey/Computer-Vision/blob/master/Neural%20Networks%20and%20CNN/Deep%20Learning%20Overview.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/anshupandey/Computer-Vision/blob/master/Transfer%20Learning%20for%20CNNs/Transfer_Learning.pptx</t>
+  </si>
+  <si>
+    <t>Transfer Learning for computer vision</t>
+  </si>
+  <si>
+    <t>word2vec</t>
+  </si>
+  <si>
+    <t>transfer learning for NLP</t>
+  </si>
+  <si>
+    <t>Attention based network, transformers</t>
+  </si>
+  <si>
+    <t>RNN &amp; LSTM</t>
+  </si>
+  <si>
+    <t>https://github.com/anshupandey/Natural_language_Processing/blob/master/NLP%20-%20Deep%20Learning%20-%20RNN%20%26%20LSTM/RNN.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/anshupandey/Natural_language_Processing/blob/master/NLP%20-%20Deep%20Learning%20-%20RNN%20%26%20LSTM/Word2vec.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/anshupandey/Natural_language_Processing/blob/master/NLP%20-%20Transfer%20Learning/Transformer%20Model.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/anshupandey/Natural_language_Processing/blob/master/NLP%20-%20Transfer%20Learning/Transfer%20Learning%20in%20NLP.pptx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +113,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,7 +437,52 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{AFEE6A29-21F1-405B-A3ED-CD51C680D3CC}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{B7003183-94B7-440D-9655-8D53C4EBE48C}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{606CA8F9-AFF8-4BD9-B7C6-8E799A36A591}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>